<commit_message>
add the ngHO calibration maps Emap/Lmap
</commit_message>
<xml_diff>
--- a/patch.xlsx
+++ b/patch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amohamed/ownCloud/HO/Lmapper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amohamed/ownCloud/HO/generalMapper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8FFD8C-43E5-1D45-ACA2-3B90FB221C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21765012-B783-B24E-A866-A42B89658EBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160" activeTab="2" xr2:uid="{6A360163-BD91-AF46-8948-2088F963F6B1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160" activeTab="6" xr2:uid="{6A360163-BD91-AF46-8948-2088F963F6B1}"/>
   </bookViews>
   <sheets>
     <sheet name="uhtr_side_c23" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="376">
   <si>
     <t>1-0-07</t>
   </si>
@@ -1132,7 +1132,40 @@
     <t xml:space="preserve">        XX_</t>
   </si>
   <si>
-    <t>XX</t>
+    <t>HO2M10 RM5</t>
+  </si>
+  <si>
+    <t>HO2M08 RM5</t>
+  </si>
+  <si>
+    <t>HO2M06 RM5</t>
+  </si>
+  <si>
+    <t>HO2M04 RM5</t>
+  </si>
+  <si>
+    <t>HO2M02 RM5</t>
+  </si>
+  <si>
+    <t>HO2M12 RM5</t>
+  </si>
+  <si>
+    <t>HO2P12 RM5</t>
+  </si>
+  <si>
+    <t>HO2P10 RM5</t>
+  </si>
+  <si>
+    <t>HO2P08 RM5</t>
+  </si>
+  <si>
+    <t>HO2P06 RM5</t>
+  </si>
+  <si>
+    <t>HO2P04 RM5</t>
+  </si>
+  <si>
+    <t>HO2P02 RM5</t>
   </si>
 </sst>
 </file>
@@ -2284,7 +2317,7 @@
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2418,7 +2451,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>30</v>
@@ -2528,7 +2561,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>31</v>
@@ -2638,7 +2671,7 @@
         <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>108</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>32</v>
@@ -2748,7 +2781,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>33</v>
@@ -2858,7 +2891,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>108</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>34</v>
@@ -2968,7 +3001,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>35</v>
@@ -3073,8 +3106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{156222D9-5E08-0146-BC7F-85A291EE069D}">
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3208,7 +3241,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>30</v>
@@ -3318,7 +3351,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>31</v>
@@ -3428,7 +3461,7 @@
         <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>108</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>32</v>
@@ -3538,7 +3571,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>33</v>
@@ -3648,7 +3681,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>108</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>34</v>
@@ -3758,7 +3791,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>35</v>
@@ -3864,7 +3897,7 @@
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5580,7 +5613,7 @@
         <v>297</v>
       </c>
       <c r="E2" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="F2" t="s">
         <v>297</v>
@@ -5800,7 +5833,7 @@
         <v>299</v>
       </c>
       <c r="E4" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F4" t="s">
         <v>299</v>
@@ -5910,7 +5943,7 @@
         <v>300</v>
       </c>
       <c r="E5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="F5" t="s">
         <v>300</v>
@@ -6020,7 +6053,7 @@
         <v>301</v>
       </c>
       <c r="E6" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="F6" t="s">
         <v>301</v>
@@ -6130,7 +6163,7 @@
         <v>302</v>
       </c>
       <c r="E7" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="F7" t="s">
         <v>302</v>
@@ -6235,8 +6268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCF09FB-4DFD-3343-9B4A-00E9E8DEA517}">
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6370,7 +6403,7 @@
         <v>330</v>
       </c>
       <c r="E2" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="F2" t="s">
         <v>330</v>
@@ -6480,7 +6513,7 @@
         <v>331</v>
       </c>
       <c r="E3" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="F3" t="s">
         <v>331</v>
@@ -6590,7 +6623,7 @@
         <v>332</v>
       </c>
       <c r="E4" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="F4" t="s">
         <v>332</v>
@@ -6700,7 +6733,7 @@
         <v>333</v>
       </c>
       <c r="E5" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="F5" t="s">
         <v>333</v>
@@ -6810,7 +6843,7 @@
         <v>334</v>
       </c>
       <c r="E6" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="F6" t="s">
         <v>334</v>
@@ -6920,7 +6953,7 @@
         <v>335</v>
       </c>
       <c r="E7" t="s">
-        <v>364</v>
+        <v>375</v>
       </c>
       <c r="F7" t="s">
         <v>335</v>

</xml_diff>